<commit_message>
we have done new change
</commit_message>
<xml_diff>
--- a/Calculator TIMER.xlsx
+++ b/Calculator TIMER.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">TIM_CLK</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">CNT_CLK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARR</t>
   </si>
   <si>
     <t xml:space="preserve">TIME IN SEC</t>
@@ -135,7 +132,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -172,14 +169,10 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>0.001</v>

</xml_diff>

<commit_message>
2nd change has been done with branch
</commit_message>
<xml_diff>
--- a/Calculator TIMER.xlsx
+++ b/Calculator TIMER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dado\Desktop\WITTE CODE\mynewonw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06860E51-9328-444A-AFDE-6F3CC7799F24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2433977E-860B-4F88-9945-F13F6A557EE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>TIM_CLK</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>TIME IN SEC</t>
+  </si>
+  <si>
+    <t>casd</t>
   </si>
 </sst>
 </file>
@@ -396,7 +399,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,6 +432,11 @@
         <v>2000000</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>

</xml_diff>